<commit_message>
Vendor Items & Stock Work Completed
</commit_message>
<xml_diff>
--- a/Table Structure.xlsx
+++ b/Table Structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Node\Payment-Records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60AEECEF-C58A-4CC7-B6A3-5FDA46AF1408}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC98DE22-2AEA-4060-8EE6-E36A562471BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{BC1AD6E1-B5BF-432E-BF54-B361662FA112}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Page</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>ItemCategory</t>
   </si>
   <si>
@@ -102,13 +99,52 @@
   </si>
   <si>
     <t>Customer Invoice Transaction Route</t>
+  </si>
+  <si>
+    <t>Invoice</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>vendor / customer</t>
+  </si>
+  <si>
+    <t>InvoiceItems</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Invoice.id</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>To be work on Customer Area , as worked on Vendor Area</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,6 +170,29 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -166,12 +225,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13361C8F-36D5-4D61-B81F-3F71F3981006}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -498,121 +560,186 @@
     <col min="2" max="2" width="22.21875" style="2" customWidth="1"/>
     <col min="3" max="3" width="36.44140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="29" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="2"/>
+    <col min="5" max="5" width="4.33203125" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E4" s="6"/>
+      <c r="F4" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E5" s="6"/>
+      <c r="F5" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B7" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="2" t="s">
+      <c r="E8" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E9" s="6"/>
+      <c r="F9" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="E10" s="6"/>
+      <c r="F10" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E11" s="6"/>
+      <c r="F11" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B13" s="3" t="s">
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="5"/>
+      <c r="B13" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C14" s="2" t="s">
+      <c r="C13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C15" s="2" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C16" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C17" s="2" t="s">
+      <c r="F16" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C18" s="2" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B20" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B22" s="2" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C22" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D22" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C23" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="D23" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C24" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C25" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C26" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>